<commit_message>
Add missing dimension tables to code table spreadsheet, handle code value conversions
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="24" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
     <sheet name="PersonEthnicityType" sheetId="50" r:id="rId2"/>
     <sheet name="PersonRaceType" sheetId="31" r:id="rId3"/>
-    <sheet name="PersonAgeType" sheetId="4" r:id="rId4"/>
-    <sheet name="PersonAgeRangeType" sheetId="25" r:id="rId5"/>
+    <sheet name="PersonAgeRangeType" sheetId="25" r:id="rId4"/>
+    <sheet name="PersonAgeType" sheetId="4" r:id="rId5"/>
     <sheet name="Facility" sheetId="33" r:id="rId6"/>
     <sheet name="Agency" sheetId="34" r:id="rId7"/>
     <sheet name="AssessmentCategoryType" sheetId="35" r:id="rId8"/>
@@ -35,8 +35,11 @@
     <sheet name="EducationLevelType" sheetId="53" r:id="rId26"/>
     <sheet name="OccupationType" sheetId="54" r:id="rId27"/>
     <sheet name="PopulationType" sheetId="55" r:id="rId28"/>
+    <sheet name="TreatmentProviderType" sheetId="57" r:id="rId29"/>
+    <sheet name="BehavioralHealthEvaluationType" sheetId="58" r:id="rId30"/>
+    <sheet name="MedicationType" sheetId="59" r:id="rId31"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="289">
   <si>
     <t>Asian</t>
   </si>
@@ -805,6 +808,114 @@
   </si>
   <si>
     <t>ChargeType 7</t>
+  </si>
+  <si>
+    <t>TreatmentProviderTypeID</t>
+  </si>
+  <si>
+    <t>TreatmentProviderTypeDescription</t>
+  </si>
+  <si>
+    <t>Provider 1</t>
+  </si>
+  <si>
+    <t>Provider 2</t>
+  </si>
+  <si>
+    <t>Provider 3</t>
+  </si>
+  <si>
+    <t>Provider 4</t>
+  </si>
+  <si>
+    <t>Provider 5</t>
+  </si>
+  <si>
+    <t>Provider 6</t>
+  </si>
+  <si>
+    <t>Provider 7</t>
+  </si>
+  <si>
+    <t>Provider 8</t>
+  </si>
+  <si>
+    <t>Provider 9</t>
+  </si>
+  <si>
+    <t>Provider 10</t>
+  </si>
+  <si>
+    <t>BehavioralHealthEvaluationTypeID</t>
+  </si>
+  <si>
+    <t>BehavioralHealthEvaluationTypeDescription</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 1</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 2</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 3</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 4</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 5</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 6</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 7</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 8</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 9</t>
+  </si>
+  <si>
+    <t>Diagnosis Category 10</t>
+  </si>
+  <si>
+    <t>MedicationTypeID</t>
+  </si>
+  <si>
+    <t>MedicationTypeDescription</t>
+  </si>
+  <si>
+    <t>Medication 1</t>
+  </si>
+  <si>
+    <t>Medication 2</t>
+  </si>
+  <si>
+    <t>Medication 3</t>
+  </si>
+  <si>
+    <t>Medication 4</t>
+  </si>
+  <si>
+    <t>Medication 5</t>
+  </si>
+  <si>
+    <t>Medication 6</t>
+  </si>
+  <si>
+    <t>Medication 7</t>
+  </si>
+  <si>
+    <t>Medication 8</t>
+  </si>
+  <si>
+    <t>Medication 9</t>
+  </si>
+  <si>
+    <t>Medication 10</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3324,7 +3435,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3370,6 +3481,129 @@
         <v>99999</v>
       </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>99998</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99999</v>
+      </c>
+      <c r="B13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3463,7 +3697,475 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>99998</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99999</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>99998</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99999</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>99998</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>99999</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C113"/>
   <sheetViews>
@@ -4724,228 +5426,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>99998</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>99999</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Accommodate staging person unique ID; tweaks to dimensional summary tables
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="24" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="297">
   <si>
     <t>Asian</t>
   </si>
@@ -916,6 +916,30 @@
   </si>
   <si>
     <t>Medication 10</t>
+  </si>
+  <si>
+    <t>ChargeTypeCitation</t>
+  </si>
+  <si>
+    <t>Citation 1</t>
+  </si>
+  <si>
+    <t>Citation 2</t>
+  </si>
+  <si>
+    <t>Citation 3</t>
+  </si>
+  <si>
+    <t>Citation 4</t>
+  </si>
+  <si>
+    <t>Citation 5</t>
+  </si>
+  <si>
+    <t>Citation 6</t>
+  </si>
+  <si>
+    <t>Citation 7</t>
   </si>
 </sst>
 </file>
@@ -1440,94 +1464,127 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3824,7 +3881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add category columns for Agency, JurisdictionType, BondStatusType, and BondType
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="313">
   <si>
     <t>Asian</t>
   </si>
@@ -940,6 +940,54 @@
   </si>
   <si>
     <t>Citation 7</t>
+  </si>
+  <si>
+    <t>BondTypeCategory</t>
+  </si>
+  <si>
+    <t>BondType Category 1</t>
+  </si>
+  <si>
+    <t>BondType Category 2</t>
+  </si>
+  <si>
+    <t>BondStatusTypeCategory</t>
+  </si>
+  <si>
+    <t>BondStatus Category 1</t>
+  </si>
+  <si>
+    <t>BondStatus Category 2</t>
+  </si>
+  <si>
+    <t>BondStatus Category 3</t>
+  </si>
+  <si>
+    <t>AgencyCategory</t>
+  </si>
+  <si>
+    <t>Agency Category 1</t>
+  </si>
+  <si>
+    <t>Agency Category 2</t>
+  </si>
+  <si>
+    <t>Agency Category 3</t>
+  </si>
+  <si>
+    <t>Agency Category 4</t>
+  </si>
+  <si>
+    <t>Agency Category 5</t>
+  </si>
+  <si>
+    <t>JurisdictionCategory</t>
+  </si>
+  <si>
+    <t>JurisdictionType Category 1</t>
+  </si>
+  <si>
+    <t>JurisdictionType Category 2</t>
   </si>
 </sst>
 </file>
@@ -1395,64 +1443,83 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1466,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1830,136 +1897,182 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="35.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>99998</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>99999</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5546,112 +5659,149 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>99998</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>99999</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5716,80 +5866,105 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="41" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added category columns for CaseStatusType and ChargeDispositionType
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="23" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="320">
   <si>
     <t>Asian</t>
   </si>
@@ -988,6 +988,27 @@
   </si>
   <si>
     <t>JurisdictionType Category 2</t>
+  </si>
+  <si>
+    <t>Charge Disposition Category A</t>
+  </si>
+  <si>
+    <t>Charge Disposition Category B</t>
+  </si>
+  <si>
+    <t>Charge Disposition Category C</t>
+  </si>
+  <si>
+    <t>CaseStatusTypeCategory</t>
+  </si>
+  <si>
+    <t>Case Status Category A</t>
+  </si>
+  <si>
+    <t>Case Status Category B</t>
+  </si>
+  <si>
+    <t>ChargeDispositionTypeCategory</t>
   </si>
 </sst>
 </file>
@@ -3110,119 +3131,159 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>99998</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>99999</v>
       </c>
       <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3233,119 +3294,159 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>213</v>
       </c>
       <c r="B1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>99998</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>99999</v>
       </c>
       <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5661,7 +5762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add SMI dimension, update a few code table extra columns
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="324">
   <si>
     <t>Asian</t>
   </si>
@@ -1009,6 +1009,18 @@
   </si>
   <si>
     <t>ChargeDispositionTypeCategory</t>
+  </si>
+  <si>
+    <t>BehavioralHealthEvaluationTypeCode</t>
+  </si>
+  <si>
+    <t>No Diagnosis</t>
+  </si>
+  <si>
+    <t>MedicationTypeCategory</t>
+  </si>
+  <si>
+    <t>MedicationTypeCode</t>
   </si>
 </sst>
 </file>
@@ -3970,119 +3982,159 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="53.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>265</v>
       </c>
       <c r="B1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>99998</v>
       </c>
       <c r="B12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>99999</v>
       </c>
       <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4093,119 +4145,199 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>277</v>
       </c>
       <c r="B1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>99998</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>99999</v>
       </c>
       <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhanced AssessmentCategoryType code table to test allegations dimension situation for Pima
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" firstSheet="23" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11535" tabRatio="663" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="330">
   <si>
     <t>Asian</t>
   </si>
@@ -1024,6 +1024,21 @@
   </si>
   <si>
     <t>BehavioralHealthEvaluationTypeCategory</t>
+  </si>
+  <si>
+    <t>AssessmentCategoryType 2</t>
+  </si>
+  <si>
+    <t>AssessmentCategoryType 3</t>
+  </si>
+  <si>
+    <t>AssessmentCategoryType 4</t>
+  </si>
+  <si>
+    <t>AssessmentCategoryType 5</t>
+  </si>
+  <si>
+    <t>AssessmentCategoryType 6</t>
   </si>
 </sst>
 </file>
@@ -3987,7 +4002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -6089,10 +6104,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6111,26 +6126,66 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>99998</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>99999</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor edits to a few code tables, and read open text staging values from dimensional code table labels
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1300" windowWidth="28940" windowHeight="14980" tabRatio="663" firstSheet="25" activeTab="30"/>
+    <workbookView xWindow="5520" yWindow="1305" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="25" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -1269,14 +1269,14 @@
       <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1335,15 +1335,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -1447,18 +1447,18 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
@@ -1587,14 +1587,14 @@
       <selection activeCell="A6" sqref="A6:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1669,14 +1669,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1735,15 +1735,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1839,14 +1839,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1921,14 +1921,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -1995,14 +1995,14 @@
       <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1">
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1">
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1">
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1">
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1">
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:2" customFormat="1">
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1">
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
@@ -2101,14 +2101,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -2183,14 +2183,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -2249,14 +2249,14 @@
       <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2323,14 +2323,14 @@
       <selection activeCell="A7" sqref="A7:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -2413,14 +2413,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2487,14 +2487,14 @@
       <selection activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>78</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2561,14 +2561,14 @@
       <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2635,14 +2635,14 @@
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>99998</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>99999</v>
       </c>
@@ -2771,14 +2771,14 @@
       <selection activeCell="A6" sqref="A6:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -2870,16 +2870,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99998</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>99999</v>
       </c>
@@ -2958,16 +2958,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>99998</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99999</v>
       </c>
@@ -3033,13 +3033,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>99998</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>99999</v>
       </c>
@@ -3097,13 +3097,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -3177,14 +3177,14 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -3263,19 +3263,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>99998</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>99999</v>
       </c>
@@ -3653,19 +3653,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>99998</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>99999</v>
       </c>
@@ -3894,13 +3894,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>99998</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>99999</v>
       </c>
@@ -4116,14 +4116,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>99998</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>99998</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>99999</v>
       </c>
@@ -5385,14 +5385,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -5459,15 +5459,15 @@
       <selection activeCell="B2" sqref="B2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -5563,14 +5563,14 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -5653,15 +5653,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>

</xml_diff>

<commit_message>
Changed Jurisdiction, Agency and Assessment codes
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1305" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="25" activeTab="29"/>
+    <workbookView xWindow="14340" yWindow="2540" windowWidth="25440" windowHeight="14980" tabRatio="663" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="260">
   <si>
     <t>Asian</t>
   </si>
@@ -399,18 +399,6 @@
     <t>Stillwater Detention Facility</t>
   </si>
   <si>
-    <t>Brookfield Police Department</t>
-  </si>
-  <si>
-    <t>Clark County Sheriff</t>
-  </si>
-  <si>
-    <t>Potsdam Police Department</t>
-  </si>
-  <si>
-    <t>Camden County Sheriff</t>
-  </si>
-  <si>
     <t>Posted Bond</t>
   </si>
   <si>
@@ -747,12 +735,6 @@
     <t>Substance Abuse</t>
   </si>
   <si>
-    <t>Psychotic</t>
-  </si>
-  <si>
-    <t>Delusional</t>
-  </si>
-  <si>
     <t>Valium</t>
   </si>
   <si>
@@ -808,6 +790,45 @@
   </si>
   <si>
     <t>Theft and Robbery</t>
+  </si>
+  <si>
+    <t>Brookfield County Sheriff</t>
+  </si>
+  <si>
+    <t>Logan City PD</t>
+  </si>
+  <si>
+    <t>Scriba City PD</t>
+  </si>
+  <si>
+    <t>Edwards City PD</t>
+  </si>
+  <si>
+    <t>Allentown Parks/Recreation Dept</t>
+  </si>
+  <si>
+    <t>Morgan College Campus Police</t>
+  </si>
+  <si>
+    <t>Brookfield County Superior Court</t>
+  </si>
+  <si>
+    <t>Logan Municipal Court</t>
+  </si>
+  <si>
+    <t>Scriba Municipal Court</t>
+  </si>
+  <si>
+    <t>Danger To Self</t>
+  </si>
+  <si>
+    <t>Danger To Others</t>
+  </si>
+  <si>
+    <t>Gravely Disabled</t>
+  </si>
+  <si>
+    <t>Persistently and Acutely Disabled</t>
   </si>
 </sst>
 </file>
@@ -863,7 +884,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -908,8 +929,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13"/>
@@ -919,8 +944,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="48">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -949,6 +977,8 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -963,6 +993,8 @@
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="13"/>
   </cellStyles>
@@ -1269,14 +1301,14 @@
       <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1284,7 +1316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1292,7 +1324,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1300,7 +1332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1308,7 +1340,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1335,15 +1367,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1354,62 +1386,62 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -1420,7 +1452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -1450,15 +1482,15 @@
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1469,84 +1501,84 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
@@ -1557,7 +1589,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
@@ -1587,14 +1619,14 @@
       <selection activeCell="A6" sqref="A6:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -1602,39 +1634,39 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1642,7 +1674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1669,14 +1701,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1684,23 +1716,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1708,7 +1740,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1729,21 +1761,21 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1754,69 +1786,58 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>99998</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
-        <v>99998</v>
+        <v>99999</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>99999</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1839,14 +1860,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1854,31 +1875,31 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1886,7 +1907,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1894,7 +1915,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1921,14 +1942,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -1936,31 +1957,31 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -1968,7 +1989,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -1995,14 +2016,14 @@
       <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -2010,63 +2031,63 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" customFormat="1">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
@@ -2074,7 +2095,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
@@ -2101,14 +2122,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -2116,39 +2137,39 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -2156,7 +2177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -2183,14 +2204,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -2198,23 +2219,23 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -2222,7 +2243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -2249,14 +2270,14 @@
       <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2264,7 +2285,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2272,7 +2293,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2280,7 +2301,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2288,7 +2309,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2296,7 +2317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2323,14 +2344,14 @@
       <selection activeCell="A7" sqref="A7:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
@@ -2338,47 +2359,47 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -2386,7 +2407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -2413,14 +2434,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
@@ -2428,31 +2449,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2460,7 +2481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2487,14 +2508,14 @@
       <selection activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>78</v>
       </c>
@@ -2502,31 +2523,31 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2534,7 +2555,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2561,14 +2582,14 @@
       <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -2576,31 +2597,31 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2608,7 +2629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2635,14 +2656,14 @@
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2653,84 +2674,84 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>99998</v>
       </c>
@@ -2741,7 +2762,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>99999</v>
       </c>
@@ -2771,14 +2792,14 @@
       <selection activeCell="A6" sqref="A6:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -2789,51 +2810,51 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -2844,7 +2865,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -2873,13 +2894,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2887,39 +2908,39 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2927,7 +2948,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>99998</v>
       </c>
@@ -2935,7 +2956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>99999</v>
       </c>
@@ -2961,13 +2982,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2975,31 +2996,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>99998</v>
       </c>
@@ -3007,7 +3028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>99999</v>
       </c>
@@ -3033,13 +3054,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3047,7 +3068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3055,7 +3076,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3063,7 +3084,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>99998</v>
       </c>
@@ -3071,7 +3092,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>99999</v>
       </c>
@@ -3097,13 +3118,13 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -3111,39 +3132,39 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -3151,7 +3172,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -3177,14 +3198,14 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3192,7 +3213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3200,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3208,7 +3229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3216,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -3224,7 +3245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3232,7 +3253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -3240,7 +3261,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -3263,19 +3284,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -3289,329 +3310,329 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C20" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D20" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C21" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D23" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>99998</v>
       </c>
@@ -3625,7 +3646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>99999</v>
       </c>
@@ -3657,15 +3678,15 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -3679,175 +3700,175 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C11" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" t="s">
         <v>242</v>
       </c>
-      <c r="C12" t="s">
-        <v>248</v>
-      </c>
       <c r="D12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C13" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D13" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>99998</v>
       </c>
@@ -3861,7 +3882,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>99999</v>
       </c>
@@ -3894,13 +3915,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3911,7 +3932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3922,7 +3943,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3933,7 +3954,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3944,7 +3965,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3955,7 +3976,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3966,7 +3987,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3977,7 +3998,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3988,7 +4009,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3999,7 +4020,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4010,7 +4031,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -4021,7 +4042,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -4032,7 +4053,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -4043,7 +4064,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -4054,7 +4075,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -4065,7 +4086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4076,7 +4097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="6">
         <v>99998</v>
       </c>
@@ -4087,7 +4108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="6">
         <v>99999</v>
       </c>
@@ -4116,14 +4137,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4134,7 +4155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4145,7 +4166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4156,7 +4177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4167,7 +4188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4178,7 +4199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4189,7 +4210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4200,7 +4221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4211,7 +4232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4222,7 +4243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4233,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4244,7 +4265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4255,7 +4276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4266,7 +4287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4277,7 +4298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4288,7 +4309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4299,7 +4320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4310,7 +4331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4321,7 +4342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4332,7 +4353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4343,7 +4364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4354,7 +4375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4365,7 +4386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4376,7 +4397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4387,7 +4408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4398,7 +4419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4409,7 +4430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4420,7 +4441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4431,7 +4452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4442,7 +4463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4453,7 +4474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4464,7 +4485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4475,7 +4496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4486,7 +4507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4497,7 +4518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4508,7 +4529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4519,7 +4540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4530,7 +4551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4541,7 +4562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4552,7 +4573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4563,7 +4584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4574,7 +4595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4585,7 +4606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4596,7 +4617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4607,7 +4628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4618,7 +4639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4629,7 +4650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4640,7 +4661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4651,7 +4672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4662,7 +4683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4673,7 +4694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4684,7 +4705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4695,7 +4716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4706,7 +4727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4717,7 +4738,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4728,7 +4749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4739,7 +4760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4750,7 +4771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4761,7 +4782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4772,7 +4793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4783,7 +4804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4794,7 +4815,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4805,7 +4826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4816,7 +4837,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4827,7 +4848,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4838,7 +4859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4849,7 +4870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4860,7 +4881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4871,7 +4892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4882,7 +4903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4893,7 +4914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4904,7 +4925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4915,7 +4936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4926,7 +4947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4937,7 +4958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4948,7 +4969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4959,7 +4980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4970,7 +4991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4981,7 +5002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4992,7 +5013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5003,7 +5024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5014,7 +5035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5025,7 +5046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5036,7 +5057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5047,7 +5068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5058,7 +5079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5069,7 +5090,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5080,7 +5101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5091,7 +5112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5102,7 +5123,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5113,7 +5134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5124,7 +5145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5135,7 +5156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5146,7 +5167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5157,7 +5178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5168,7 +5189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5179,7 +5200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5190,7 +5211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5201,7 +5222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5212,7 +5233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5223,7 +5244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5234,7 +5255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5245,7 +5266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5256,7 +5277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5267,7 +5288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5278,7 +5299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5289,7 +5310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5300,7 +5321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5311,7 +5332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5322,7 +5343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5333,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5344,7 +5365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112">
         <v>99998</v>
       </c>
@@ -5355,7 +5376,7 @@
         <v>99998</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113">
         <v>99999</v>
       </c>
@@ -5385,14 +5406,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -5400,7 +5421,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5408,7 +5429,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5416,7 +5437,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5424,7 +5445,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -5432,7 +5453,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -5453,21 +5474,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -5478,69 +5499,91 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>119</v>
+      <c r="B5" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
         <v>99998</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
         <v>99999</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5557,20 +5600,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -5578,59 +5621,67 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="8" spans="1:2">
+      <c r="A8" s="2">
         <v>99998</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
         <v>99999</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5653,15 +5704,15 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -5672,62 +5723,62 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -5738,7 +5789,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>99999</v>
       </c>

</xml_diff>

<commit_message>
A little tidying of code tables
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14980" tabRatio="663" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="23" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="267">
   <si>
     <t>Asian</t>
   </si>
@@ -408,9 +408,6 @@
     <t>No Charges</t>
   </si>
   <si>
-    <t>CASH</t>
-  </si>
-  <si>
     <t>Served Time Release</t>
   </si>
   <si>
@@ -447,24 +444,6 @@
     <t>Traffic</t>
   </si>
   <si>
-    <t>Alcohol Related</t>
-  </si>
-  <si>
-    <t>Assault And Battery</t>
-  </si>
-  <si>
-    <t>Driving And Traffic</t>
-  </si>
-  <si>
-    <t>Drug</t>
-  </si>
-  <si>
-    <t>Sex Crimes</t>
-  </si>
-  <si>
-    <t>Fraud and Financial</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -501,48 +480,18 @@
     <t>Retired</t>
   </si>
   <si>
-    <t>Housing</t>
-  </si>
-  <si>
-    <t>Drug Rehab</t>
-  </si>
-  <si>
-    <t>Alcohol Rehab</t>
-  </si>
-  <si>
-    <t>Family Counseling</t>
-  </si>
-  <si>
     <t>Not Registered</t>
   </si>
   <si>
     <t>Registered</t>
   </si>
   <si>
-    <t>General</t>
-  </si>
-  <si>
     <t>Adult</t>
   </si>
   <si>
     <t>Juvenile</t>
   </si>
   <si>
-    <t>Solitary</t>
-  </si>
-  <si>
-    <t>Substance Abuse Treatment</t>
-  </si>
-  <si>
-    <t>Self</t>
-  </si>
-  <si>
-    <t>Court</t>
-  </si>
-  <si>
-    <t>Prescribed-Diagnosed</t>
-  </si>
-  <si>
     <t>Not Active</t>
   </si>
   <si>
@@ -582,27 +531,6 @@
     <t>Post-Secondary</t>
   </si>
   <si>
-    <t>Professional</t>
-  </si>
-  <si>
-    <t>Unskilled</t>
-  </si>
-  <si>
-    <t>Skilled</t>
-  </si>
-  <si>
-    <t>Psychologist</t>
-  </si>
-  <si>
-    <t>Social Worker</t>
-  </si>
-  <si>
-    <t>Counselor</t>
-  </si>
-  <si>
-    <t>Therapist</t>
-  </si>
-  <si>
     <t>Drug Dependence</t>
   </si>
   <si>
@@ -780,12 +708,6 @@
     <t>Homeless</t>
   </si>
   <si>
-    <t>Homeless-Veteran</t>
-  </si>
-  <si>
-    <t>Theft and Robbery</t>
-  </si>
-  <si>
     <t>Brookfield County Sheriff</t>
   </si>
   <si>
@@ -826,6 +748,108 @@
   </si>
   <si>
     <t>Brookfield County Detention Center</t>
+  </si>
+  <si>
+    <t>Housing Assistance</t>
+  </si>
+  <si>
+    <t>TANF</t>
+  </si>
+  <si>
+    <t>Job Placement Services</t>
+  </si>
+  <si>
+    <t>Isolation</t>
+  </si>
+  <si>
+    <t>Medical</t>
+  </si>
+  <si>
+    <t>Court-ordered</t>
+  </si>
+  <si>
+    <t>Other involuntary</t>
+  </si>
+  <si>
+    <t>Voluntary</t>
+  </si>
+  <si>
+    <t>Non-Homeless</t>
+  </si>
+  <si>
+    <t>Criminal Homicide</t>
+  </si>
+  <si>
+    <t>Forcible Rape</t>
+  </si>
+  <si>
+    <t>Robbery</t>
+  </si>
+  <si>
+    <t>Aggravated Assault</t>
+  </si>
+  <si>
+    <t>Burglary</t>
+  </si>
+  <si>
+    <t>Larceny / Theft</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft</t>
+  </si>
+  <si>
+    <t>Arson</t>
+  </si>
+  <si>
+    <t>Drug Crimes</t>
+  </si>
+  <si>
+    <t>Citation 8</t>
+  </si>
+  <si>
+    <t>Citation 9</t>
+  </si>
+  <si>
+    <t>Brookfield Counseling Center</t>
+  </si>
+  <si>
+    <t>Westside Behavioral Health</t>
+  </si>
+  <si>
+    <t>Logan Interfaith Family Resources</t>
+  </si>
+  <si>
+    <t>Downtown Psychiatric Associates</t>
+  </si>
+  <si>
+    <t>Unemployed</t>
+  </si>
+  <si>
+    <t>Professional/Technical/Related</t>
+  </si>
+  <si>
+    <t>Executive/Managerial</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Administrative Support</t>
+  </si>
+  <si>
+    <t>Precision Production/Craft/Repair</t>
+  </si>
+  <si>
+    <t>Machine Operator/Assembler</t>
+  </si>
+  <si>
+    <t>Transportation / Material Moving</t>
+  </si>
+  <si>
+    <t>Handlers/Helpers/Laborers</t>
+  </si>
+  <si>
+    <t>Service Occupations</t>
   </si>
 </sst>
 </file>
@@ -1306,14 +1330,14 @@
       <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1321,7 +1345,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1329,7 +1353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1337,7 +1361,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1345,7 +1369,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1372,15 +1396,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1391,40 +1415,40 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1432,21 +1456,21 @@
         <v>115</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -1457,7 +1481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -1481,21 +1505,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1506,102 +1530,124 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>242</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>133</v>
+        <v>243</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>244</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>137</v>
+        <v>248</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>99998</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>99999</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1624,14 +1670,14 @@
       <selection activeCell="A6" sqref="A6:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -1639,39 +1685,39 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1679,7 +1725,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1703,17 +1749,17 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1721,23 +1767,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1745,7 +1791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1768,19 +1814,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1791,40 +1837,40 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -1835,7 +1881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -1865,14 +1911,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1880,31 +1926,31 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1912,7 +1958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1920,7 +1966,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1947,14 +1993,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -1962,31 +2008,31 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -1994,7 +2040,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2021,14 +2067,14 @@
       <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -2036,63 +2082,63 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1">
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" customFormat="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" customFormat="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" customFormat="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" customFormat="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
@@ -2100,7 +2146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
@@ -2121,20 +2167,20 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -2142,51 +2188,43 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>99998</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>99998</v>
+        <v>99999</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2">
-        <v>99999</v>
-      </c>
-      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2209,14 +2247,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -2224,23 +2262,23 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -2248,7 +2286,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -2275,14 +2313,14 @@
       <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2290,7 +2328,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2298,7 +2336,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2306,7 +2344,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2314,7 +2352,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2322,7 +2360,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2343,20 +2381,20 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD11"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
@@ -2364,59 +2402,51 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>99998</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>99998</v>
+        <v>99999</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2">
-        <v>99999</v>
-      </c>
-      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2433,20 +2463,20 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
@@ -2454,43 +2484,51 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>99998</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>99999</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2513,14 +2551,14 @@
       <selection activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>78</v>
       </c>
@@ -2528,31 +2566,31 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2560,7 +2598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2587,14 +2625,14 @@
       <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -2602,31 +2640,31 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2634,7 +2672,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2661,14 +2699,14 @@
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2679,40 +2717,40 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2723,40 +2761,40 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>99998</v>
       </c>
@@ -2767,7 +2805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>99999</v>
       </c>
@@ -2797,14 +2835,14 @@
       <selection activeCell="A6" sqref="A6:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -2815,29 +2853,29 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2848,18 +2886,18 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -2870,7 +2908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -2899,13 +2937,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2913,39 +2951,39 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2953,7 +2991,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99998</v>
       </c>
@@ -2961,7 +2999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>99999</v>
       </c>
@@ -2981,19 +3019,19 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3001,43 +3039,99 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>99998</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>99999</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3059,13 +3153,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3073,7 +3167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3081,7 +3175,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3089,7 +3183,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>99998</v>
       </c>
@@ -3097,7 +3191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>99999</v>
       </c>
@@ -3120,16 +3214,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -3137,39 +3231,39 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -3177,7 +3271,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -3203,14 +3297,14 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3218,7 +3312,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3226,7 +3320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3234,7 +3328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3242,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -3250,7 +3344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3258,7 +3352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -3266,7 +3360,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -3293,15 +3387,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -3315,329 +3409,329 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="D11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="D16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="D20" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="C22" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="D22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="C23" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C24" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>99998</v>
       </c>
@@ -3651,7 +3745,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>99999</v>
       </c>
@@ -3683,15 +3777,15 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -3705,175 +3799,175 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="D12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="C13" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>99998</v>
       </c>
@@ -3887,7 +3981,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>99999</v>
       </c>
@@ -3920,13 +4014,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3937,7 +4031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3948,7 +4042,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3959,7 +4053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3970,7 +4064,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3981,7 +4075,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3992,7 +4086,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4003,7 +4097,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4014,7 +4108,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -4025,7 +4119,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4036,7 +4130,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -4047,7 +4141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -4058,7 +4152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -4069,7 +4163,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -4080,7 +4174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -4091,7 +4185,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4102,7 +4196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>99998</v>
       </c>
@@ -4113,7 +4207,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>99999</v>
       </c>
@@ -4142,14 +4236,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4160,7 +4254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4171,7 +4265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4182,7 +4276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4193,7 +4287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4204,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4215,7 +4309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4226,7 +4320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4237,7 +4331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4248,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4259,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4270,7 +4364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4281,7 +4375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4292,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4303,7 +4397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4314,7 +4408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4325,7 +4419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4336,7 +4430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4347,7 +4441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4358,7 +4452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4369,7 +4463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4380,7 +4474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4391,7 +4485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4402,7 +4496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4413,7 +4507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4424,7 +4518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4435,7 +4529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4446,7 +4540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4457,7 +4551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4468,7 +4562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4479,7 +4573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4490,7 +4584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4501,7 +4595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4512,7 +4606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4523,7 +4617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4534,7 +4628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4545,7 +4639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4556,7 +4650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4567,7 +4661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4578,7 +4672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4589,7 +4683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4600,7 +4694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4611,7 +4705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4622,7 +4716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4633,7 +4727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4644,7 +4738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4655,7 +4749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4666,7 +4760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4677,7 +4771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4688,7 +4782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4699,7 +4793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4710,7 +4804,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4721,7 +4815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4732,7 +4826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4743,7 +4837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4754,7 +4848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4765,7 +4859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4776,7 +4870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4787,7 +4881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4798,7 +4892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4809,7 +4903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4820,7 +4914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4831,7 +4925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4842,7 +4936,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4853,7 +4947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4864,7 +4958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4875,7 +4969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4886,7 +4980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4897,7 +4991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4908,7 +5002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4919,7 +5013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4930,7 +5024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4941,7 +5035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4952,7 +5046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4963,7 +5057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4974,7 +5068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4985,7 +5079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4996,7 +5090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5007,7 +5101,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5018,7 +5112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5029,7 +5123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5040,7 +5134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5051,7 +5145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5062,7 +5156,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5073,7 +5167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5084,7 +5178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5095,7 +5189,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5106,7 +5200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5117,7 +5211,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5128,7 +5222,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5139,7 +5233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5150,7 +5244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5161,7 +5255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5172,7 +5266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5183,7 +5277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5194,7 +5288,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5205,7 +5299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5216,7 +5310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5227,7 +5321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5238,7 +5332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5249,7 +5343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5260,7 +5354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5271,7 +5365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5282,7 +5376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5293,7 +5387,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5304,7 +5398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5315,7 +5409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5326,7 +5420,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5337,7 +5431,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5348,7 +5442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5359,7 +5453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5370,7 +5464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>99998</v>
       </c>
@@ -5381,7 +5475,7 @@
         <v>99998</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>99999</v>
       </c>
@@ -5411,14 +5505,14 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -5426,15 +5520,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5442,7 +5536,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -5450,7 +5544,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -5477,15 +5571,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -5496,73 +5590,73 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99998</v>
       </c>
@@ -5573,7 +5667,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>99999</v>
       </c>
@@ -5603,14 +5697,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -5618,47 +5712,47 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5666,7 +5760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99998</v>
       </c>
@@ -5674,7 +5768,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>99999</v>
       </c>
@@ -5698,18 +5792,18 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -5720,7 +5814,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5731,7 +5825,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5742,18 +5836,18 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5764,18 +5858,18 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -5786,7 +5880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>99999</v>
       </c>

</xml_diff>

<commit_message>
Improved medication dimension table values
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="23" activeTab="26"/>
+    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="25" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="265">
   <si>
     <t>Asian</t>
   </si>
@@ -531,9 +531,6 @@
     <t>Post-Secondary</t>
   </si>
   <si>
-    <t>Drug Dependence</t>
-  </si>
-  <si>
     <t>Anxiety Disorders</t>
   </si>
   <si>
@@ -657,54 +654,6 @@
     <t>Substance Abuse</t>
   </si>
   <si>
-    <t>Valium</t>
-  </si>
-  <si>
-    <t>Ativan</t>
-  </si>
-  <si>
-    <t>Zoluft</t>
-  </si>
-  <si>
-    <t>Lexapro</t>
-  </si>
-  <si>
-    <t>Dolophine</t>
-  </si>
-  <si>
-    <t>Suboxone</t>
-  </si>
-  <si>
-    <t>Librium</t>
-  </si>
-  <si>
-    <t>Zyprexa</t>
-  </si>
-  <si>
-    <t>Luvox</t>
-  </si>
-  <si>
-    <t>Cogentin</t>
-  </si>
-  <si>
-    <t>Psychosis</t>
-  </si>
-  <si>
-    <t>Antideprin</t>
-  </si>
-  <si>
-    <t>Major Depressive Disorder</t>
-  </si>
-  <si>
-    <t>Subutex</t>
-  </si>
-  <si>
-    <t>Anxiety disorders</t>
-  </si>
-  <si>
-    <t>Bipolar Disorder</t>
-  </si>
-  <si>
     <t>Homeless</t>
   </si>
   <si>
@@ -850,6 +799,51 @@
   </si>
   <si>
     <t>Service Occupations</t>
+  </si>
+  <si>
+    <t>Diazepam</t>
+  </si>
+  <si>
+    <t>Antianxiety Medications</t>
+  </si>
+  <si>
+    <t>Lorazepam</t>
+  </si>
+  <si>
+    <t>Sertraline</t>
+  </si>
+  <si>
+    <t>Antidepressants</t>
+  </si>
+  <si>
+    <t>Fluoxetine</t>
+  </si>
+  <si>
+    <t>Trimipramine</t>
+  </si>
+  <si>
+    <t>Clozapine</t>
+  </si>
+  <si>
+    <t>Antipsychotics</t>
+  </si>
+  <si>
+    <t>Olanzapine</t>
+  </si>
+  <si>
+    <t>Methadone</t>
+  </si>
+  <si>
+    <t>Substance Abuse Treatment</t>
+  </si>
+  <si>
+    <t>Naltrexone</t>
+  </si>
+  <si>
+    <t>Disulfiram</t>
+  </si>
+  <si>
+    <t>Acamprosate</t>
   </si>
 </sst>
 </file>
@@ -1535,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>95</v>
@@ -1546,7 +1540,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>96</v>
@@ -1557,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>97</v>
@@ -1568,7 +1562,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>98</v>
@@ -1579,7 +1573,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>99</v>
@@ -1590,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>100</v>
@@ -1601,7 +1595,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>101</v>
@@ -1612,10 +1606,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1623,10 +1617,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1780,7 +1774,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1842,10 +1836,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1853,10 +1847,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1864,10 +1858,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2193,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,7 +2195,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2209,7 +2203,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2423,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2425,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2489,7 +2483,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2497,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2505,7 +2499,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3021,8 +3015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3052,7 +3046,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3060,7 +3054,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3068,7 +3062,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3076,7 +3070,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3084,7 +3078,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3092,7 +3086,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3100,7 +3094,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,7 +3102,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3116,7 +3110,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3236,7 +3230,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3244,7 +3238,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3252,7 +3246,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3260,7 +3254,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3414,13 +3408,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
         <v>161</v>
       </c>
-      <c r="C2" t="s">
-        <v>162</v>
-      </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3428,13 +3422,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
         <v>163</v>
       </c>
-      <c r="C3" t="s">
-        <v>164</v>
-      </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3442,13 +3436,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" t="s">
         <v>165</v>
       </c>
-      <c r="C4" t="s">
-        <v>166</v>
-      </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3456,13 +3450,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
         <v>167</v>
       </c>
-      <c r="C5" t="s">
-        <v>168</v>
-      </c>
       <c r="D5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,13 +3464,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
         <v>169</v>
       </c>
-      <c r="C6" t="s">
-        <v>170</v>
-      </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3484,13 +3478,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
         <v>171</v>
       </c>
-      <c r="C7" t="s">
-        <v>172</v>
-      </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3498,13 +3492,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" t="s">
         <v>173</v>
       </c>
-      <c r="C8" t="s">
-        <v>174</v>
-      </c>
       <c r="D8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,13 +3506,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3526,13 +3520,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" t="s">
         <v>176</v>
       </c>
-      <c r="C10" t="s">
-        <v>177</v>
-      </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,13 +3534,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" t="s">
         <v>178</v>
       </c>
-      <c r="C11" t="s">
-        <v>179</v>
-      </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,13 +3548,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
         <v>180</v>
       </c>
-      <c r="C12" t="s">
-        <v>181</v>
-      </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,13 +3562,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
         <v>182</v>
       </c>
-      <c r="C13" t="s">
-        <v>183</v>
-      </c>
       <c r="D13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3582,13 +3576,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" t="s">
         <v>184</v>
       </c>
-      <c r="C14" t="s">
-        <v>185</v>
-      </c>
       <c r="D14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,13 +3590,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3610,13 +3604,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3624,13 +3618,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3638,13 +3632,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" t="s">
         <v>189</v>
       </c>
-      <c r="C18" t="s">
-        <v>190</v>
-      </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3652,13 +3646,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3666,13 +3660,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" t="s">
         <v>192</v>
       </c>
-      <c r="C20" t="s">
-        <v>193</v>
-      </c>
       <c r="D20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3680,13 +3674,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" t="s">
         <v>194</v>
       </c>
-      <c r="C21" t="s">
-        <v>195</v>
-      </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3694,13 +3688,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" t="s">
         <v>196</v>
       </c>
-      <c r="C22" t="s">
-        <v>197</v>
-      </c>
       <c r="D22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3708,13 +3702,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>197</v>
+      </c>
+      <c r="C23" t="s">
         <v>198</v>
       </c>
-      <c r="C23" t="s">
-        <v>199</v>
-      </c>
       <c r="D23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,13 +3716,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3771,17 +3765,17 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3804,13 +3798,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3818,13 +3812,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3832,27 +3826,27 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>258</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>213</v>
+      <c r="B5" t="s">
+        <v>259</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>258</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3860,13 +3854,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
-        <v>214</v>
+        <v>261</v>
       </c>
       <c r="D6" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3874,13 +3868,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>262</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>261</v>
       </c>
       <c r="D7" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3888,13 +3882,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>263</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>261</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3902,27 +3896,27 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>264</v>
       </c>
       <c r="C9" t="s">
-        <v>160</v>
+        <v>261</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>208</v>
+      <c r="B10" s="8" t="s">
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" t="s">
-        <v>161</v>
+        <v>254</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3930,13 +3924,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>255</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>254</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3944,54 +3938,40 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s">
-        <v>216</v>
+        <v>254</v>
       </c>
       <c r="D12" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>99998</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>212</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>99998</v>
+        <v>99999</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>99999</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5525,7 +5505,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5595,10 +5575,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5606,10 +5586,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5617,10 +5597,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5628,7 +5608,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
@@ -5639,7 +5619,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>28</v>
@@ -5650,7 +5630,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>28</v>
@@ -5717,7 +5697,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5725,7 +5705,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5733,7 +5713,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5741,7 +5721,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5749,7 +5729,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implement Charge Class Category in dimensional DB, mondrian schema, and code tables
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="25" activeTab="30"/>
+    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="266">
   <si>
     <t>Asian</t>
   </si>
@@ -844,6 +844,9 @@
   </si>
   <si>
     <t>Acamprosate</t>
+  </si>
+  <si>
+    <t>ChargeClassTypeCategory</t>
   </si>
 </sst>
 </file>
@@ -1658,72 +1661,94 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="27.85546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3767,7 +3792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Support code tables with different logical/physical names; add BehavioralHealthInvolvementIndicator to booking view
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="25" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="TreatmentProviderType" sheetId="57" r:id="rId29"/>
     <sheet name="BehavioralHealthEvaluationType" sheetId="58" r:id="rId30"/>
     <sheet name="MedicationType" sheetId="59" r:id="rId31"/>
+    <sheet name="IndicatorType" sheetId="60" r:id="rId32"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="270">
   <si>
     <t>Asian</t>
   </si>
@@ -847,6 +848,18 @@
   </si>
   <si>
     <t>ChargeClassTypeCategory</t>
+  </si>
+  <si>
+    <t>IndicatorTypeID</t>
+  </si>
+  <si>
+    <t>IndicatorTypeDescription</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4011,6 +4024,49 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>

</xml_diff>

<commit_message>
updating charge categories so there is repitition
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/git/analytics/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1800" windowWidth="25440" windowHeight="14985" tabRatio="663" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="3020" yWindow="3620" windowWidth="25440" windowHeight="14980" tabRatio="663" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="32" r:id="rId1"/>
@@ -42,6 +47,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -50,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="274">
   <si>
     <t>Asian</t>
   </si>
@@ -872,24 +880,6 @@
   </si>
   <si>
     <t>Category 3</t>
-  </si>
-  <si>
-    <t>Category 4</t>
-  </si>
-  <si>
-    <t>Category 5</t>
-  </si>
-  <si>
-    <t>Category 6</t>
-  </si>
-  <si>
-    <t>Category 7</t>
-  </si>
-  <si>
-    <t>Category 8</t>
-  </si>
-  <si>
-    <t>Category 9</t>
   </si>
 </sst>
 </file>
@@ -1120,12 +1110,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1155,12 +1145,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1370,14 +1360,14 @@
       <selection activeCell="A4" sqref="A4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1385,7 +1375,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1393,7 +1383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1401,7 +1391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1409,7 +1399,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1420,11 +1410,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1436,15 +1421,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1455,7 +1440,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1466,7 +1451,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1477,7 +1462,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1488,7 +1473,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1499,7 +1484,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1510,7 +1495,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -1521,7 +1506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -1535,11 +1520,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1548,19 +1528,19 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1554,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1588,7 +1568,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1602,7 +1582,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1616,7 +1596,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1627,10 +1607,10 @@
         <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1641,10 +1621,10 @@
         <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1655,10 +1635,10 @@
         <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1669,10 +1649,10 @@
         <v>101</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1683,10 +1663,10 @@
         <v>234</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1697,10 +1677,10 @@
         <v>235</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>99998</v>
       </c>
@@ -1714,7 +1694,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>99999</v>
       </c>
@@ -1731,11 +1711,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1747,15 +1722,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -1766,7 +1741,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1777,7 +1752,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1788,7 +1763,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1799,7 +1774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1810,7 +1785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -1821,7 +1796,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -1835,11 +1810,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1851,14 +1821,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>64</v>
       </c>
@@ -1866,7 +1836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1874,7 +1844,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1882,7 +1852,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -1890,7 +1860,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -1901,11 +1871,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1917,15 +1882,15 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1936,7 +1901,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1947,7 +1912,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1958,7 +1923,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1969,7 +1934,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -1980,7 +1945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -1994,11 +1959,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2010,14 +1970,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="14.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -2025,7 +1985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2033,7 +1993,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2041,7 +2001,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2049,7 +2009,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2057,7 +2017,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -2065,7 +2025,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -2076,11 +2036,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2092,14 +2047,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
@@ -2107,7 +2062,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2115,7 +2070,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2123,7 +2078,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2131,7 +2086,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2139,7 +2094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2150,11 +2105,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2166,14 +2116,14 @@
       <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>68</v>
       </c>
@@ -2181,7 +2131,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2189,7 +2139,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2197,7 +2147,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2205,7 +2155,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2213,7 +2163,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2221,7 +2171,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2229,7 +2179,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2237,7 +2187,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>99998</v>
       </c>
@@ -2245,7 +2195,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>99999</v>
       </c>
@@ -2256,11 +2206,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2272,14 +2217,14 @@
       <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -2287,7 +2232,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2295,7 +2240,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2303,7 +2248,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2311,7 +2256,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2319,7 +2264,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2330,11 +2275,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2346,14 +2286,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>72</v>
       </c>
@@ -2361,7 +2301,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2369,7 +2309,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2377,7 +2317,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -2385,7 +2325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -2396,11 +2336,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2412,14 +2347,14 @@
       <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2427,7 +2362,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2435,7 +2370,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2443,7 +2378,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2451,7 +2386,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2459,7 +2394,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2470,11 +2405,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2486,14 +2416,14 @@
       <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
@@ -2501,7 +2431,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2509,7 +2439,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2517,7 +2447,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2525,7 +2455,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2533,7 +2463,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -2541,7 +2471,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -2552,11 +2482,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2568,14 +2493,14 @@
       <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="30.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>76</v>
       </c>
@@ -2583,7 +2508,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2591,7 +2516,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2599,7 +2524,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2607,7 +2532,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2615,7 +2540,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99998</v>
       </c>
@@ -2623,7 +2548,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99999</v>
       </c>
@@ -2634,11 +2559,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2650,14 +2570,14 @@
       <selection activeCell="A5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>78</v>
       </c>
@@ -2665,7 +2585,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2673,7 +2593,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2681,7 +2601,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2689,7 +2609,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2697,7 +2617,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2708,11 +2628,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2724,14 +2639,14 @@
       <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>80</v>
       </c>
@@ -2739,7 +2654,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2747,7 +2662,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2755,7 +2670,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2763,7 +2678,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99998</v>
       </c>
@@ -2771,7 +2686,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>99999</v>
       </c>
@@ -2782,11 +2697,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2798,14 +2708,14 @@
       <selection activeCell="B5" sqref="B5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2816,7 +2726,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2827,7 +2737,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2838,7 +2748,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2849,7 +2759,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2860,7 +2770,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2871,7 +2781,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2882,7 +2792,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2893,7 +2803,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>99998</v>
       </c>
@@ -2904,7 +2814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>99999</v>
       </c>
@@ -2918,11 +2828,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2934,14 +2839,14 @@
       <selection activeCell="A6" sqref="A6:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -2952,7 +2857,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2963,7 +2868,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2974,7 +2879,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2985,7 +2890,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2996,7 +2901,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -3007,7 +2912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -3020,11 +2925,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3036,13 +2936,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -3050,7 +2950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3058,7 +2958,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3066,7 +2966,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3074,7 +2974,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3082,7 +2982,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3090,7 +2990,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>99998</v>
       </c>
@@ -3098,7 +2998,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>99999</v>
       </c>
@@ -3108,11 +3008,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3124,13 +3019,13 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3138,7 +3033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3146,7 +3041,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3154,7 +3049,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3162,7 +3057,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3170,7 +3065,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3178,7 +3073,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3186,7 +3081,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3194,7 +3089,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3202,7 +3097,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3210,7 +3105,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3218,7 +3113,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>99998</v>
       </c>
@@ -3226,7 +3121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>99999</v>
       </c>
@@ -3236,11 +3131,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3252,13 +3142,13 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -3266,7 +3156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3274,7 +3164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3282,7 +3172,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>99998</v>
       </c>
@@ -3290,7 +3180,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>99999</v>
       </c>
@@ -3300,11 +3190,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3316,13 +3201,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -3330,7 +3215,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3338,7 +3223,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3346,7 +3231,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3354,7 +3239,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3362,7 +3247,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>99998</v>
       </c>
@@ -3370,7 +3255,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>99999</v>
       </c>
@@ -3380,11 +3265,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3396,14 +3276,14 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3411,7 +3291,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3419,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3427,7 +3307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3435,7 +3315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -3443,7 +3323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3451,7 +3331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -3459,7 +3339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -3470,11 +3350,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3486,15 +3361,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -3508,7 +3383,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3522,7 +3397,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3536,7 +3411,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3550,7 +3425,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3564,7 +3439,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3578,7 +3453,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3592,7 +3467,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3606,7 +3481,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3620,7 +3495,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3634,7 +3509,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3648,7 +3523,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3662,7 +3537,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3676,7 +3551,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3690,7 +3565,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3704,7 +3579,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3718,7 +3593,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3732,7 +3607,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3746,7 +3621,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3760,7 +3635,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3774,7 +3649,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3788,7 +3663,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3802,7 +3677,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3816,7 +3691,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3830,7 +3705,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>99998</v>
       </c>
@@ -3844,7 +3719,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>99999</v>
       </c>
@@ -3860,11 +3735,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3876,15 +3746,15 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -3898,7 +3768,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3912,7 +3782,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3926,7 +3796,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3940,7 +3810,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3954,7 +3824,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3968,7 +3838,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3982,7 +3852,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3996,7 +3866,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4010,7 +3880,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4024,7 +3894,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4038,7 +3908,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4052,7 +3922,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>99998</v>
       </c>
@@ -4066,7 +3936,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>99999</v>
       </c>
@@ -4083,11 +3953,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4099,13 +3964,13 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>266</v>
       </c>
@@ -4113,7 +3978,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4121,7 +3986,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4142,13 +4007,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -4159,7 +4024,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4170,7 +4035,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4181,7 +4046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4192,7 +4057,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4203,7 +4068,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4214,7 +4079,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4225,7 +4090,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4236,7 +4101,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -4247,7 +4112,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4258,7 +4123,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -4269,7 +4134,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -4280,7 +4145,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -4291,7 +4156,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -4302,7 +4167,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -4313,7 +4178,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4324,7 +4189,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>99998</v>
       </c>
@@ -4335,7 +4200,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>99999</v>
       </c>
@@ -4348,11 +4213,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4364,14 +4224,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4382,7 +4242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4393,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4404,7 +4264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4415,7 +4275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4426,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4437,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4448,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4459,7 +4319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4470,7 +4330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4481,7 +4341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4492,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4503,7 +4363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4514,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4525,7 +4385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4536,7 +4396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4547,7 +4407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4558,7 +4418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4569,7 +4429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4580,7 +4440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4591,7 +4451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4602,7 +4462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4613,7 +4473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4624,7 +4484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4635,7 +4495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4646,7 +4506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4657,7 +4517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4668,7 +4528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4679,7 +4539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4690,7 +4550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4701,7 +4561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4712,7 +4572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4723,7 +4583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4734,7 +4594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4745,7 +4605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4756,7 +4616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4767,7 +4627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4778,7 +4638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4789,7 +4649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4800,7 +4660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4811,7 +4671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4822,7 +4682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4833,7 +4693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4844,7 +4704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4855,7 +4715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4866,7 +4726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4877,7 +4737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4888,7 +4748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4899,7 +4759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4910,7 +4770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4921,7 +4781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4932,7 +4792,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4943,7 +4803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4954,7 +4814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4965,7 +4825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4976,7 +4836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4987,7 +4847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4998,7 +4858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5009,7 +4869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5020,7 +4880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5031,7 +4891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5042,7 +4902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5053,7 +4913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5064,7 +4924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5075,7 +4935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5086,7 +4946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5097,7 +4957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5108,7 +4968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5119,7 +4979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5130,7 +4990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5141,7 +5001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5152,7 +5012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5163,7 +5023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5174,7 +5034,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5185,7 +5045,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5196,7 +5056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5207,7 +5067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5218,7 +5078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5229,7 +5089,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5240,7 +5100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5251,7 +5111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5262,7 +5122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5273,7 +5133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5284,7 +5144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5295,7 +5155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5306,7 +5166,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5317,7 +5177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5328,7 +5188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5339,7 +5199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5350,7 +5210,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5361,7 +5221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5372,7 +5232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5383,7 +5243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5394,7 +5254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5405,7 +5265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5416,7 +5276,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5427,7 +5287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5438,7 +5298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5449,7 +5309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5460,7 +5320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5471,7 +5331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5482,7 +5342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5493,7 +5353,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5504,7 +5364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5515,7 +5375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5526,7 +5386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5537,7 +5397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5548,7 +5408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5559,7 +5419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5570,7 +5430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5581,7 +5441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5592,7 +5452,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>99998</v>
       </c>
@@ -5603,7 +5463,7 @@
         <v>99998</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>99999</v>
       </c>
@@ -5617,11 +5477,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5633,14 +5488,14 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="10.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -5648,7 +5503,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5656,7 +5511,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5664,7 +5519,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>99998</v>
       </c>
@@ -5672,7 +5527,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>99999</v>
       </c>
@@ -5683,11 +5538,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5699,15 +5549,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
@@ -5718,7 +5568,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5729,7 +5579,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5740,7 +5590,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5751,7 +5601,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5762,7 +5612,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -5773,7 +5623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -5784,7 +5634,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>99998</v>
       </c>
@@ -5795,7 +5645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>99999</v>
       </c>
@@ -5809,11 +5659,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5825,14 +5670,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="24.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -5840,7 +5685,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5848,7 +5693,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5856,7 +5701,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5864,7 +5709,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5872,7 +5717,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5880,7 +5725,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5888,7 +5733,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>99998</v>
       </c>
@@ -5896,7 +5741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>99999</v>
       </c>
@@ -5907,11 +5752,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5923,15 +5763,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -5942,7 +5782,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5953,7 +5793,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5964,7 +5804,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5975,7 +5815,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5986,7 +5826,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5997,7 +5837,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>99998</v>
       </c>
@@ -6008,7 +5848,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>99999</v>
       </c>
@@ -6022,10 +5862,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add booking classification dimension to loading and db
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
+++ b/booking-jail/r-load/OJBCJailBookingLoad/inst/raw/DimensionalCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="855" firstSheet="26" activeTab="36"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="855" firstSheet="28" activeTab="37"/>
   </bookViews>
   <sheets>
     <sheet name="PersonSexType" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,7 @@
     <sheet name="DispositionLocationType" sheetId="35" r:id="rId35"/>
     <sheet name="RespondingUnitType" sheetId="36" r:id="rId36"/>
     <sheet name="TimeSpanType" sheetId="37" r:id="rId37"/>
+    <sheet name="BookingClassificationType" sheetId="38" r:id="rId38"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="313">
   <si>
     <t>PersonSexTypeID</t>
   </si>
@@ -985,6 +986,15 @@
   </si>
   <si>
     <t>2AM-6:30AM</t>
+  </si>
+  <si>
+    <t>BookingClassificationTypeID</t>
+  </si>
+  <si>
+    <t>BookingClassificationTypeDescription</t>
+  </si>
+  <si>
+    <t>BookingClassificationTypeCategory</t>
   </si>
 </sst>
 </file>
@@ -4377,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4432,6 +4442,59 @@
         <v>99999</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>99998</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>99999</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>